<commit_message>
Mostly layout changes. Filters added. EndDate added to Promo but not yet in pre_pos.zul (TODO) Empty Dart to support empty line in darts combobox in pre_pos.zul
</commit_message>
<xml_diff>
--- a/service/src/test/resources/templates/Pricelist.xlsx
+++ b/service/src/test/resources/templates/Pricelist.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\cisco\service\src\test\resources\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -65,8 +60,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,6 +129,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -196,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,7 +229,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,28 +406,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +441,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -456,8 +456,9 @@
       <c r="D2" s="3">
         <v>37</v>
       </c>
+      <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -470,8 +471,9 @@
       <c r="D3" s="3">
         <v>37</v>
       </c>
+      <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -484,8 +486,9 @@
       <c r="D4" s="5">
         <v>37</v>
       </c>
+      <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -498,8 +501,10 @@
       <c r="D5" s="6">
         <v>42</v>
       </c>
+      <c r="E5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>